<commit_message>
importacion masiva - cambios en el template
</commit_message>
<xml_diff>
--- a/src/Sofco.WebApi/wwwroot/excelTemplates/worktime-template.xlsx
+++ b/src/Sofco.WebApi/wwwroot/excelTemplates/worktime-template.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Recursos" sheetId="1" r:id="rId1"/>
+    <sheet name="Tareas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Recurso</t>
   </si>
@@ -25,9 +26,6 @@
     <t>Fecha</t>
   </si>
   <si>
-    <t>Descripcion Tarea</t>
-  </si>
-  <si>
     <t>Id Tarea</t>
   </si>
   <si>
@@ -35,6 +33,15 @@
   </si>
   <si>
     <t>Comentarios</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Tarea</t>
+  </si>
+  <si>
+    <t>Código</t>
   </si>
 </sst>
 </file>
@@ -76,10 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,11 +404,10 @@
     <col min="2" max="2" width="44.140625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" customWidth="1"/>
+    <col min="6" max="6" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -411,22 +418,50 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D363"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
baja de recursos- eliminacion de asignaciones
</commit_message>
<xml_diff>
--- a/src/Sofco.WebApi/wwwroot/excelTemplates/worktime-template.xlsx
+++ b/src/Sofco.WebApi/wwwroot/excelTemplates/worktime-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Recursos" sheetId="1" r:id="rId1"/>
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D363"/>
     </sheetView>
   </sheetViews>

</xml_diff>